<commit_message>
Edition des reçus fonctionnelle
</commit_message>
<xml_diff>
--- a/donnees/listesAdherents/2023.xlsx
+++ b/donnees/listesAdherents/2023.xlsx
@@ -586,7 +586,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>Cary</t>
+          <t>CARY</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -594,7 +594,11 @@
           <t>André</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr"/>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>231231AC0</t>
+        </is>
+      </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -655,7 +659,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>Tamalout</t>
+          <t>TAMALOUT</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -663,7 +667,11 @@
           <t>Alexandre</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr"/>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>231231AT0</t>
+        </is>
+      </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -724,7 +732,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Provost</t>
+          <t>PROVOST</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -732,7 +740,11 @@
           <t>Vincent</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr"/>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>231231VP0</t>
+        </is>
+      </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -793,7 +805,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Prevost</t>
+          <t>PREVOST</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -801,7 +813,11 @@
           <t>Arthur</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr"/>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>231231AP0</t>
+        </is>
+      </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -862,7 +878,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Julien</t>
+          <t>JULIEN</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -870,7 +886,11 @@
           <t>Marion</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr"/>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>231231MJ0</t>
+        </is>
+      </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -931,7 +951,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Maurice</t>
+          <t>MAURICE</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -939,7 +959,11 @@
           <t>Matilda</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr"/>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>231231MM0</t>
+        </is>
+      </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1000,7 +1024,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Vincent</t>
+          <t>VINCENT</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -1008,7 +1032,11 @@
           <t>Véronique</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr"/>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>231231VV0</t>
+        </is>
+      </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1069,7 +1097,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Boulanger</t>
+          <t>BOULANGER</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -1077,7 +1105,11 @@
           <t>Ludivine</t>
         </is>
       </c>
-      <c r="D9" s="3" t="inlineStr"/>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>231231LB0</t>
+        </is>
+      </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1138,7 +1170,7 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Pasteur</t>
+          <t>PASTEUR</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -1146,7 +1178,11 @@
           <t>Thérèse</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr"/>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>231231TP0</t>
+        </is>
+      </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1207,15 +1243,19 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Pastier</t>
+          <t>PASTIER</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>Jean-Pierre</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="inlineStr"/>
+          <t>Jean-pierre</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>231231JP0</t>
+        </is>
+      </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1276,7 +1316,7 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>Rucher</t>
+          <t>RUCHER</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -1284,7 +1324,11 @@
           <t>Francis</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr"/>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>231231FR0</t>
+        </is>
+      </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1345,7 +1389,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>Tison</t>
+          <t>TISON</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -1353,7 +1397,11 @@
           <t>Gisèle</t>
         </is>
       </c>
-      <c r="D13" s="3" t="inlineStr"/>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>231231GT0</t>
+        </is>
+      </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1414,7 +1462,7 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>Tresseau</t>
+          <t>TRESSEAU</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -1422,7 +1470,11 @@
           <t>Yves</t>
         </is>
       </c>
-      <c r="D14" s="3" t="inlineStr"/>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>231231YT0</t>
+        </is>
+      </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1483,7 +1535,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Morgan</t>
+          <t>MORGAN</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -1491,7 +1543,11 @@
           <t>Gilles</t>
         </is>
       </c>
-      <c r="D15" s="3" t="inlineStr"/>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>231231GM0</t>
+        </is>
+      </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1552,7 +1608,7 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Leclerc</t>
+          <t>LECLERC</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -1560,7 +1616,11 @@
           <t>Léa</t>
         </is>
       </c>
-      <c r="D16" s="3" t="inlineStr"/>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>231231LL0</t>
+        </is>
+      </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1621,7 +1681,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>Solognot</t>
+          <t>SOLOGNOT</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -1629,7 +1689,11 @@
           <t>Léo</t>
         </is>
       </c>
-      <c r="D17" s="3" t="inlineStr"/>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>231231LS0</t>
+        </is>
+      </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1690,7 +1754,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>Zanzibar</t>
+          <t>ZANZIBAR</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -1698,7 +1762,11 @@
           <t>Maurice</t>
         </is>
       </c>
-      <c r="D18" s="3" t="inlineStr"/>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>231231MZ0</t>
+        </is>
+      </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1759,7 +1827,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>NORMAL</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1767,7 +1835,11 @@
           <t>Patrice</t>
         </is>
       </c>
-      <c r="D19" s="3" t="inlineStr"/>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>231231PN0</t>
+        </is>
+      </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1828,7 +1900,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Froid</t>
+          <t>FROID</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1836,7 +1908,11 @@
           <t>Patricia</t>
         </is>
       </c>
-      <c r="D20" s="3" t="inlineStr"/>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>231231PF0</t>
+        </is>
+      </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1897,7 +1973,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Chaud</t>
+          <t>CHAUD</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1905,7 +1981,11 @@
           <t>Henri</t>
         </is>
       </c>
-      <c r="D21" s="3" t="inlineStr"/>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>231231HC0</t>
+        </is>
+      </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -1966,7 +2046,7 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Tiède</t>
+          <t>TIÈDE</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1974,7 +2054,11 @@
           <t>Alice</t>
         </is>
       </c>
-      <c r="D22" s="3" t="inlineStr"/>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>231231AT0</t>
+        </is>
+      </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -2035,7 +2119,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>Temperet</t>
+          <t>TEMPERET</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -2043,7 +2127,11 @@
           <t>Véronique</t>
         </is>
       </c>
-      <c r="D23" s="3" t="inlineStr"/>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>231231VT0</t>
+        </is>
+      </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -2104,7 +2192,7 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Parasol</t>
+          <t>PARASOL</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -2112,7 +2200,11 @@
           <t>Nathalie</t>
         </is>
       </c>
-      <c r="D24" s="3" t="inlineStr"/>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>231231NP0</t>
+        </is>
+      </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
           <t>NA</t>
@@ -2173,15 +2265,19 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>Baignoire</t>
+          <t>BAIGNOIRE</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>Jean-Pierre</t>
-        </is>
-      </c>
-      <c r="D25" s="3" t="inlineStr"/>
+          <t>Jean-pierre</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>231231JB0</t>
+        </is>
+      </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
           <t>NA</t>

</xml_diff>

<commit_message>
Gestion des doublons d'identifiants --> ID unique Les PDFs sont bien (re)-générés seulement si besoin (nouveau paiement ou paiement modifié) Sauvegarde des paiements (identifiant, hash et refPaiement pour chacun). Permet le fonctionnement des deux fonctionnalités du dessus. Ajout du texte "ID du reçu : " avant d'inscrire l'identifiant dans le PDF
</commit_message>
<xml_diff>
--- a/donnees/listesAdherents/2023.xlsx
+++ b/donnees/listesAdherents/2023.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -80,12 +78,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -579,1756 +576,1756 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>nj76@mail.com</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>CARY</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>André</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>231231AC0</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>231231AC1</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="b">
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>17 rue du hamster</t>
         </is>
       </c>
-      <c r="I2" s="3" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>38000</t>
         </is>
       </c>
-      <c r="J2" s="3" t="inlineStr">
+      <c r="J2" s="2" t="inlineStr">
         <is>
           <t>Grenoble</t>
         </is>
       </c>
-      <c r="K2" s="3" t="inlineStr"/>
-      <c r="L2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="3" t="inlineStr">
+      <c r="K2" s="2" t="inlineStr"/>
+      <c r="L2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R2" s="3" t="inlineStr">
+      <c r="R2" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S2" s="3" t="n"/>
+      <c r="S2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>joj98@mail.com</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>TAMALOUT</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>Alexandre</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>231231AT0</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>231231AT2</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="b">
+      <c r="F3" s="2" t="n"/>
+      <c r="G3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="H3" s="2" t="inlineStr">
         <is>
           <t>18 rue du lapin</t>
         </is>
       </c>
-      <c r="I3" s="3" t="inlineStr">
+      <c r="I3" s="2" t="inlineStr">
         <is>
           <t>38000</t>
         </is>
       </c>
-      <c r="J3" s="3" t="inlineStr">
+      <c r="J3" s="2" t="inlineStr">
         <is>
           <t>GRENOBLE</t>
         </is>
       </c>
-      <c r="K3" s="3" t="inlineStr"/>
-      <c r="L3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="3" t="inlineStr">
+      <c r="K3" s="2" t="inlineStr"/>
+      <c r="L3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R3" s="3" t="inlineStr">
+      <c r="R3" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S3" s="3" t="n"/>
+      <c r="S3" s="2" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>sd78@mail.com</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>PROVOST</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>Vincent</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>231231VP0</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>231231VP1</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F4" s="3" t="n"/>
-      <c r="G4" s="3" t="b">
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="3" t="inlineStr">
+      <c r="H4" s="2" t="inlineStr">
         <is>
           <t>19 avenue du dromadaire</t>
         </is>
       </c>
-      <c r="I4" s="3" t="inlineStr">
+      <c r="I4" s="2" t="inlineStr">
         <is>
           <t>38000</t>
         </is>
       </c>
-      <c r="J4" s="3" t="inlineStr">
+      <c r="J4" s="2" t="inlineStr">
         <is>
           <t>Grenoble</t>
         </is>
       </c>
-      <c r="K4" s="3" t="inlineStr"/>
-      <c r="L4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3" t="inlineStr">
+      <c r="K4" s="2" t="inlineStr"/>
+      <c r="L4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R4" s="3" t="inlineStr">
+      <c r="R4" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S4" s="3" t="n"/>
+      <c r="S4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>oiij78@test.fr</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>PREVOST</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>Arthur</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>231231AP0</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>231231AP1</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3" t="b">
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="3" t="inlineStr">
+      <c r="H5" s="2" t="inlineStr">
         <is>
           <t>20 rue du lapin</t>
         </is>
       </c>
-      <c r="I5" s="3" t="inlineStr">
+      <c r="I5" s="2" t="inlineStr">
         <is>
           <t>38340</t>
         </is>
       </c>
-      <c r="J5" s="3" t="inlineStr">
+      <c r="J5" s="2" t="inlineStr">
         <is>
           <t>Voreppe</t>
         </is>
       </c>
-      <c r="K5" s="3" t="inlineStr"/>
-      <c r="L5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="3" t="inlineStr">
+      <c r="K5" s="2" t="inlineStr"/>
+      <c r="L5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R5" s="3" t="inlineStr">
+      <c r="R5" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S5" s="3" t="n"/>
+      <c r="S5" s="2" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>mooj98@exemple.fr</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>JULIEN</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>Marion</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>231231MJ0</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>231231MJ1</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="b">
+      <c r="F6" s="2" t="n"/>
+      <c r="G6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="3" t="inlineStr">
+      <c r="H6" s="2" t="inlineStr">
         <is>
           <t>21 rue de la gerbille</t>
         </is>
       </c>
-      <c r="I6" s="3" t="inlineStr">
+      <c r="I6" s="2" t="inlineStr">
         <is>
           <t>38440</t>
         </is>
       </c>
-      <c r="J6" s="3" t="inlineStr">
+      <c r="J6" s="2" t="inlineStr">
         <is>
           <t>ARTAS</t>
         </is>
       </c>
-      <c r="K6" s="3" t="inlineStr"/>
-      <c r="L6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3" t="inlineStr">
+      <c r="K6" s="2" t="inlineStr"/>
+      <c r="L6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R6" s="3" t="inlineStr">
+      <c r="R6" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S6" s="3" t="n"/>
+      <c r="S6" s="2" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>jsjs65@exemple.fr</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>MAURICE</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>Matilda</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>231231MM0</t>
-        </is>
-      </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>231231MM1</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3" t="b">
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="3" t="inlineStr">
+      <c r="H7" s="2" t="inlineStr">
         <is>
           <t>22 rue du zèbre</t>
         </is>
       </c>
-      <c r="I7" s="3" t="inlineStr">
+      <c r="I7" s="2" t="inlineStr">
         <is>
           <t>38350</t>
         </is>
       </c>
-      <c r="J7" s="3" t="inlineStr">
+      <c r="J7" s="2" t="inlineStr">
         <is>
           <t>Nantes en Rattier</t>
         </is>
       </c>
-      <c r="K7" s="3" t="inlineStr"/>
-      <c r="L7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="3" t="inlineStr">
+      <c r="K7" s="2" t="inlineStr"/>
+      <c r="L7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R7" s="3" t="inlineStr">
+      <c r="R7" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S7" s="3" t="n"/>
+      <c r="S7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>bbu756@mail.com</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>VINCENT</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>Véronique</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>231231VV0</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>231231VV1</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="b">
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="3" t="inlineStr">
+      <c r="H8" s="2" t="inlineStr">
         <is>
           <t>23 rue de la gerbille</t>
         </is>
       </c>
-      <c r="I8" s="3" t="inlineStr">
+      <c r="I8" s="2" t="inlineStr">
         <is>
           <t>38600</t>
         </is>
       </c>
-      <c r="J8" s="3" t="inlineStr">
+      <c r="J8" s="2" t="inlineStr">
         <is>
           <t>fontaine</t>
         </is>
       </c>
-      <c r="K8" s="3" t="inlineStr"/>
-      <c r="L8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="3" t="inlineStr">
+      <c r="K8" s="2" t="inlineStr"/>
+      <c r="L8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R8" s="3" t="inlineStr">
+      <c r="R8" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S8" s="3" t="n"/>
+      <c r="S8" s="2" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>bbhs65@test.fr</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>BOULANGER</t>
         </is>
       </c>
-      <c r="C9" s="3" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>Ludivine</t>
         </is>
       </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>231231LB0</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>231231LB1</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F9" s="3" t="n"/>
-      <c r="G9" s="3" t="b">
+      <c r="F9" s="2" t="n"/>
+      <c r="G9" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="3" t="inlineStr">
+      <c r="H9" s="2" t="inlineStr">
         <is>
           <t>24 allée des lagomorphes</t>
         </is>
       </c>
-      <c r="I9" s="3" t="inlineStr">
+      <c r="I9" s="2" t="inlineStr">
         <is>
           <t>38640</t>
         </is>
       </c>
-      <c r="J9" s="3" t="inlineStr">
+      <c r="J9" s="2" t="inlineStr">
         <is>
           <t>CLAIX</t>
         </is>
       </c>
-      <c r="K9" s="3" t="inlineStr"/>
-      <c r="L9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3" t="inlineStr">
+      <c r="K9" s="2" t="inlineStr"/>
+      <c r="L9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R9" s="3" t="inlineStr">
+      <c r="R9" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S9" s="3" t="n"/>
+      <c r="S9" s="2" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>hdhc8@exemple.fr</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>PASTEUR</t>
         </is>
       </c>
-      <c r="C10" s="3" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>Thérèse</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>231231TP0</t>
-        </is>
-      </c>
-      <c r="E10" s="3" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>231231TP1</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F10" s="3" t="n"/>
-      <c r="G10" s="3" t="b">
+      <c r="F10" s="2" t="n"/>
+      <c r="G10" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="3" t="inlineStr">
+      <c r="H10" s="2" t="inlineStr">
         <is>
           <t>25 rue du capybara</t>
         </is>
       </c>
-      <c r="I10" s="3" t="inlineStr">
+      <c r="I10" s="2" t="inlineStr">
         <is>
           <t>38600</t>
         </is>
       </c>
-      <c r="J10" s="3" t="inlineStr">
+      <c r="J10" s="2" t="inlineStr">
         <is>
           <t>Fontaine</t>
         </is>
       </c>
-      <c r="K10" s="3" t="inlineStr"/>
-      <c r="L10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="3" t="inlineStr">
+      <c r="K10" s="2" t="inlineStr"/>
+      <c r="L10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R10" s="3" t="inlineStr">
+      <c r="R10" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S10" s="3" t="n"/>
+      <c r="S10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>jnjsd7@test.fr</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>PASTIER</t>
         </is>
       </c>
-      <c r="C11" s="3" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>Jean-pierre</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>231231JP0</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>231231JP1</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F11" s="3" t="n"/>
-      <c r="G11" s="3" t="b">
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="3" t="inlineStr">
+      <c r="H11" s="2" t="inlineStr">
         <is>
           <t>26 avenue du dromadaire</t>
         </is>
       </c>
-      <c r="I11" s="3" t="inlineStr">
+      <c r="I11" s="2" t="inlineStr">
         <is>
           <t>73700</t>
         </is>
       </c>
-      <c r="J11" s="3" t="inlineStr">
+      <c r="J11" s="2" t="inlineStr">
         <is>
           <t>SEEZ</t>
         </is>
       </c>
-      <c r="K11" s="3" t="inlineStr"/>
-      <c r="L11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="3" t="inlineStr">
+      <c r="K11" s="2" t="inlineStr"/>
+      <c r="L11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R11" s="3" t="inlineStr">
+      <c r="R11" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S11" s="3" t="n"/>
+      <c r="S11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>jbjsbd8@exemple.fr</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>RUCHER</t>
         </is>
       </c>
-      <c r="C12" s="3" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>Francis</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>231231FR0</t>
-        </is>
-      </c>
-      <c r="E12" s="3" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>231231FR1</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F12" s="3" t="n"/>
-      <c r="G12" s="3" t="b">
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="3" t="inlineStr">
+      <c r="H12" s="2" t="inlineStr">
         <is>
           <t>27 rue du lapin</t>
         </is>
       </c>
-      <c r="I12" s="3" t="inlineStr">
+      <c r="I12" s="2" t="inlineStr">
         <is>
           <t>38920</t>
         </is>
       </c>
-      <c r="J12" s="3" t="inlineStr">
+      <c r="J12" s="2" t="inlineStr">
         <is>
           <t>Crolles</t>
         </is>
       </c>
-      <c r="K12" s="3" t="inlineStr"/>
-      <c r="L12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="3" t="inlineStr">
+      <c r="K12" s="2" t="inlineStr"/>
+      <c r="L12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R12" s="3" t="inlineStr">
+      <c r="R12" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S12" s="3" t="n"/>
+      <c r="S12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>sjdbj786@exemple.fr</t>
         </is>
       </c>
-      <c r="B13" s="3" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>TISON</t>
         </is>
       </c>
-      <c r="C13" s="3" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>Gisèle</t>
         </is>
       </c>
-      <c r="D13" s="3" t="inlineStr">
-        <is>
-          <t>231231GT0</t>
-        </is>
-      </c>
-      <c r="E13" s="3" t="inlineStr">
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>231231GT1</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F13" s="3" t="n"/>
-      <c r="G13" s="3" t="b">
+      <c r="F13" s="2" t="n"/>
+      <c r="G13" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="3" t="inlineStr">
+      <c r="H13" s="2" t="inlineStr">
         <is>
           <t>28 allée des lagomorphes</t>
         </is>
       </c>
-      <c r="I13" s="3" t="inlineStr">
+      <c r="I13" s="2" t="inlineStr">
         <is>
           <t>38190</t>
         </is>
       </c>
-      <c r="J13" s="3" t="inlineStr">
+      <c r="J13" s="2" t="inlineStr">
         <is>
           <t>LAVAL</t>
         </is>
       </c>
-      <c r="K13" s="3" t="inlineStr"/>
-      <c r="L13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="3" t="inlineStr">
+      <c r="K13" s="2" t="inlineStr"/>
+      <c r="L13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R13" s="3" t="inlineStr">
+      <c r="R13" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S13" s="3" t="n"/>
+      <c r="S13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>bhsd112@test.fr</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>TRESSEAU</t>
         </is>
       </c>
-      <c r="C14" s="3" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>Yves</t>
         </is>
       </c>
-      <c r="D14" s="3" t="inlineStr">
-        <is>
-          <t>231231YT0</t>
-        </is>
-      </c>
-      <c r="E14" s="3" t="inlineStr">
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>231231YT1</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F14" s="3" t="n"/>
-      <c r="G14" s="3" t="b">
+      <c r="F14" s="2" t="n"/>
+      <c r="G14" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H14" s="3" t="inlineStr">
+      <c r="H14" s="2" t="inlineStr">
         <is>
           <t>29 rue du zèbre</t>
         </is>
       </c>
-      <c r="I14" s="3" t="inlineStr">
+      <c r="I14" s="2" t="inlineStr">
         <is>
           <t>38360</t>
         </is>
       </c>
-      <c r="J14" s="3" t="inlineStr">
+      <c r="J14" s="2" t="inlineStr">
         <is>
           <t>Noyarey</t>
         </is>
       </c>
-      <c r="K14" s="3" t="inlineStr"/>
-      <c r="L14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="3" t="inlineStr">
+      <c r="K14" s="2" t="inlineStr"/>
+      <c r="L14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R14" s="3" t="inlineStr">
+      <c r="R14" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S14" s="3" t="n"/>
+      <c r="S14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>jij134@exemple.fr</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>MORGAN</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>Gilles</t>
         </is>
       </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>231231GM0</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="inlineStr">
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>231231GM1</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="b">
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="3" t="inlineStr">
+      <c r="H15" s="2" t="inlineStr">
         <is>
           <t>30 rue du lapin</t>
         </is>
       </c>
-      <c r="I15" s="3" t="inlineStr">
+      <c r="I15" s="2" t="inlineStr">
         <is>
           <t>38600</t>
         </is>
       </c>
-      <c r="J15" s="3" t="inlineStr">
+      <c r="J15" s="2" t="inlineStr">
         <is>
           <t>FONTAINE</t>
         </is>
       </c>
-      <c r="K15" s="3" t="inlineStr"/>
-      <c r="L15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="3" t="inlineStr">
+      <c r="K15" s="2" t="inlineStr"/>
+      <c r="L15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R15" s="3" t="inlineStr">
+      <c r="R15" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S15" s="3" t="n"/>
+      <c r="S15" s="2" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>hu7651@test.fr</t>
         </is>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>LECLERC</t>
         </is>
       </c>
-      <c r="C16" s="3" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>Léa</t>
         </is>
       </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>231231LL0</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="inlineStr">
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>231231LL1</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F16" s="3" t="n"/>
-      <c r="G16" s="3" t="b">
+      <c r="F16" s="2" t="n"/>
+      <c r="G16" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="3" t="inlineStr">
+      <c r="H16" s="2" t="inlineStr">
         <is>
           <t>31 rue de la gerbille</t>
         </is>
       </c>
-      <c r="I16" s="3" t="inlineStr">
+      <c r="I16" s="2" t="inlineStr">
         <is>
           <t>38610</t>
         </is>
       </c>
-      <c r="J16" s="3" t="inlineStr">
+      <c r="J16" s="2" t="inlineStr">
         <is>
           <t>Gières</t>
         </is>
       </c>
-      <c r="K16" s="3" t="inlineStr"/>
-      <c r="L16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="3" t="inlineStr">
+      <c r="K16" s="2" t="inlineStr"/>
+      <c r="L16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R16" s="3" t="inlineStr">
+      <c r="R16" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S16" s="3" t="n"/>
+      <c r="S16" s="2" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>12djd@mail.com</t>
         </is>
       </c>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>SOLOGNOT</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>Léo</t>
         </is>
       </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>231231LS0</t>
-        </is>
-      </c>
-      <c r="E17" s="3" t="inlineStr">
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>231231LS1</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F17" s="3" t="n"/>
-      <c r="G17" s="3" t="b">
+      <c r="F17" s="2" t="n"/>
+      <c r="G17" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H17" s="3" t="inlineStr">
+      <c r="H17" s="2" t="inlineStr">
         <is>
           <t>32 rue du zèbre</t>
         </is>
       </c>
-      <c r="I17" s="3" t="inlineStr">
+      <c r="I17" s="2" t="inlineStr">
         <is>
           <t>69230</t>
         </is>
       </c>
-      <c r="J17" s="3" t="inlineStr">
+      <c r="J17" s="2" t="inlineStr">
         <is>
           <t>SAINT-GENIS-LAVAL</t>
         </is>
       </c>
-      <c r="K17" s="3" t="inlineStr"/>
-      <c r="L17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="3" t="inlineStr">
+      <c r="K17" s="2" t="inlineStr"/>
+      <c r="L17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R17" s="3" t="inlineStr">
+      <c r="R17" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S17" s="3" t="n"/>
+      <c r="S17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>091ssj@exemple.fr</t>
         </is>
       </c>
-      <c r="B18" s="3" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>ZANZIBAR</t>
         </is>
       </c>
-      <c r="C18" s="3" t="inlineStr">
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>Maurice</t>
         </is>
       </c>
-      <c r="D18" s="3" t="inlineStr">
-        <is>
-          <t>231231MZ0</t>
-        </is>
-      </c>
-      <c r="E18" s="3" t="inlineStr">
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>231231MZ1</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F18" s="3" t="n"/>
-      <c r="G18" s="3" t="b">
+      <c r="F18" s="2" t="n"/>
+      <c r="G18" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H18" s="3" t="inlineStr">
+      <c r="H18" s="2" t="inlineStr">
         <is>
           <t>33 rue de la gerbille</t>
         </is>
       </c>
-      <c r="I18" s="3" t="inlineStr">
+      <c r="I18" s="2" t="inlineStr">
         <is>
           <t>38110</t>
         </is>
       </c>
-      <c r="J18" s="3" t="inlineStr">
+      <c r="J18" s="2" t="inlineStr">
         <is>
           <t>MONTAGNIEU</t>
         </is>
       </c>
-      <c r="K18" s="3" t="inlineStr"/>
-      <c r="L18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="3" t="inlineStr">
+      <c r="K18" s="2" t="inlineStr"/>
+      <c r="L18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R18" s="3" t="inlineStr">
+      <c r="R18" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S18" s="3" t="n"/>
+      <c r="S18" s="2" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>art134@mail.com</t>
         </is>
       </c>
-      <c r="B19" s="3" t="inlineStr">
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>NORMAL</t>
         </is>
       </c>
-      <c r="C19" s="3" t="inlineStr">
+      <c r="C19" s="2" t="inlineStr">
         <is>
           <t>Patrice</t>
         </is>
       </c>
-      <c r="D19" s="3" t="inlineStr">
-        <is>
-          <t>231231PN0</t>
-        </is>
-      </c>
-      <c r="E19" s="3" t="inlineStr">
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>231231PN1</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F19" s="3" t="n"/>
-      <c r="G19" s="3" t="b">
+      <c r="F19" s="2" t="n"/>
+      <c r="G19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H19" s="3" t="inlineStr">
+      <c r="H19" s="2" t="inlineStr">
         <is>
           <t>34 rue du lapin</t>
         </is>
       </c>
-      <c r="I19" s="3" t="inlineStr">
+      <c r="I19" s="2" t="inlineStr">
         <is>
           <t>38120</t>
         </is>
       </c>
-      <c r="J19" s="3" t="inlineStr">
+      <c r="J19" s="2" t="inlineStr">
         <is>
           <t>Saint-Égrève</t>
         </is>
       </c>
-      <c r="K19" s="3" t="inlineStr"/>
-      <c r="L19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="3" t="inlineStr">
+      <c r="K19" s="2" t="inlineStr"/>
+      <c r="L19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R19" s="3" t="inlineStr">
+      <c r="R19" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S19" s="3" t="n"/>
+      <c r="S19" s="2" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>112ssss@mail.com</t>
         </is>
       </c>
-      <c r="B20" s="3" t="inlineStr">
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>FROID</t>
         </is>
       </c>
-      <c r="C20" s="3" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
         <is>
           <t>Patricia</t>
         </is>
       </c>
-      <c r="D20" s="3" t="inlineStr">
-        <is>
-          <t>231231PF0</t>
-        </is>
-      </c>
-      <c r="E20" s="3" t="inlineStr">
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>231231PF1</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F20" s="3" t="n"/>
-      <c r="G20" s="3" t="b">
+      <c r="F20" s="2" t="n"/>
+      <c r="G20" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H20" s="3" t="inlineStr">
+      <c r="H20" s="2" t="inlineStr">
         <is>
           <t>35 avenue du dromadaire</t>
         </is>
       </c>
-      <c r="I20" s="3" t="inlineStr">
+      <c r="I20" s="2" t="inlineStr">
         <is>
           <t>38150</t>
         </is>
       </c>
-      <c r="J20" s="3" t="inlineStr">
+      <c r="J20" s="2" t="inlineStr">
         <is>
           <t>Salaise-sur-Sanne 38150</t>
         </is>
       </c>
-      <c r="K20" s="3" t="inlineStr"/>
-      <c r="L20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="3" t="inlineStr">
+      <c r="K20" s="2" t="inlineStr"/>
+      <c r="L20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R20" s="3" t="inlineStr">
+      <c r="R20" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S20" s="3" t="n"/>
+      <c r="S20" s="2" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>uhu761@test.fr</t>
         </is>
       </c>
-      <c r="B21" s="3" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>CHAUD</t>
         </is>
       </c>
-      <c r="C21" s="3" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>Henri</t>
         </is>
       </c>
-      <c r="D21" s="3" t="inlineStr">
-        <is>
-          <t>231231HC0</t>
-        </is>
-      </c>
-      <c r="E21" s="3" t="inlineStr">
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>231231HC1</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F21" s="3" t="n"/>
-      <c r="G21" s="3" t="b">
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H21" s="3" t="inlineStr">
+      <c r="H21" s="2" t="inlineStr">
         <is>
           <t>36 rue du hamster</t>
         </is>
       </c>
-      <c r="I21" s="3" t="inlineStr">
+      <c r="I21" s="2" t="inlineStr">
         <is>
           <t>38300</t>
         </is>
       </c>
-      <c r="J21" s="3" t="inlineStr">
+      <c r="J21" s="2" t="inlineStr">
         <is>
           <t>BOURGOIN JALLIEU</t>
         </is>
       </c>
-      <c r="K21" s="3" t="inlineStr"/>
-      <c r="L21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="3" t="inlineStr">
+      <c r="K21" s="2" t="inlineStr"/>
+      <c r="L21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R21" s="3" t="inlineStr">
+      <c r="R21" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S21" s="3" t="n"/>
+      <c r="S21" s="2" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>azaz541@test.fr</t>
         </is>
       </c>
-      <c r="B22" s="3" t="inlineStr">
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>TIÈDE</t>
         </is>
       </c>
-      <c r="C22" s="3" t="inlineStr">
+      <c r="C22" s="2" t="inlineStr">
         <is>
           <t>Alice</t>
         </is>
       </c>
-      <c r="D22" s="3" t="inlineStr">
-        <is>
-          <t>231231AT0</t>
-        </is>
-      </c>
-      <c r="E22" s="3" t="inlineStr">
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>231231AT1</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F22" s="3" t="n"/>
-      <c r="G22" s="3" t="b">
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H22" s="3" t="inlineStr">
+      <c r="H22" s="2" t="inlineStr">
         <is>
           <t>37 rue du lapin</t>
         </is>
       </c>
-      <c r="I22" s="3" t="inlineStr">
+      <c r="I22" s="2" t="inlineStr">
         <is>
           <t>38610</t>
         </is>
       </c>
-      <c r="J22" s="3" t="inlineStr">
+      <c r="J22" s="2" t="inlineStr">
         <is>
           <t>Gieres</t>
         </is>
       </c>
-      <c r="K22" s="3" t="inlineStr"/>
-      <c r="L22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="3" t="inlineStr">
+      <c r="K22" s="2" t="inlineStr"/>
+      <c r="L22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R22" s="3" t="inlineStr">
+      <c r="R22" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S22" s="3" t="n"/>
+      <c r="S22" s="2" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>sjjs183@mail.com</t>
         </is>
       </c>
-      <c r="B23" s="3" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>TEMPERET</t>
         </is>
       </c>
-      <c r="C23" s="3" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>Véronique</t>
         </is>
       </c>
-      <c r="D23" s="3" t="inlineStr">
-        <is>
-          <t>231231VT0</t>
-        </is>
-      </c>
-      <c r="E23" s="3" t="inlineStr">
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>231231VT1</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F23" s="3" t="n"/>
-      <c r="G23" s="3" t="b">
+      <c r="F23" s="2" t="n"/>
+      <c r="G23" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H23" s="3" t="inlineStr">
+      <c r="H23" s="2" t="inlineStr">
         <is>
           <t>38 rue du capybara</t>
         </is>
       </c>
-      <c r="I23" s="3" t="inlineStr">
+      <c r="I23" s="2" t="inlineStr">
         <is>
           <t>38000</t>
         </is>
       </c>
-      <c r="J23" s="3" t="inlineStr">
+      <c r="J23" s="2" t="inlineStr">
         <is>
           <t>GRENOBLE</t>
         </is>
       </c>
-      <c r="K23" s="3" t="inlineStr"/>
-      <c r="L23" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="3" t="inlineStr">
+      <c r="K23" s="2" t="inlineStr"/>
+      <c r="L23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R23" s="3" t="inlineStr">
+      <c r="R23" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S23" s="3" t="n"/>
+      <c r="S23" s="2" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr">
         <is>
           <t>apn514@mail.com</t>
         </is>
       </c>
-      <c r="B24" s="3" t="inlineStr">
+      <c r="B24" s="2" t="inlineStr">
         <is>
           <t>PARASOL</t>
         </is>
       </c>
-      <c r="C24" s="3" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
         <is>
           <t>Nathalie</t>
         </is>
       </c>
-      <c r="D24" s="3" t="inlineStr">
-        <is>
-          <t>231231NP0</t>
-        </is>
-      </c>
-      <c r="E24" s="3" t="inlineStr">
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>231231NP1</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F24" s="3" t="n"/>
-      <c r="G24" s="3" t="b">
+      <c r="F24" s="2" t="n"/>
+      <c r="G24" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H24" s="3" t="inlineStr">
+      <c r="H24" s="2" t="inlineStr">
         <is>
           <t>39 rue de la gerbille</t>
         </is>
       </c>
-      <c r="I24" s="3" t="inlineStr">
+      <c r="I24" s="2" t="inlineStr">
         <is>
           <t>38000</t>
         </is>
       </c>
-      <c r="J24" s="3" t="inlineStr">
+      <c r="J24" s="2" t="inlineStr">
         <is>
           <t>GRENOBLE</t>
         </is>
       </c>
-      <c r="K24" s="3" t="inlineStr"/>
-      <c r="L24" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="3" t="inlineStr">
+      <c r="K24" s="2" t="inlineStr"/>
+      <c r="L24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R24" s="3" t="inlineStr">
+      <c r="R24" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S24" s="3" t="n"/>
+      <c r="S24" s="2" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>jijsq12@mail.com</t>
         </is>
       </c>
-      <c r="B25" s="3" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>BAIGNOIRE</t>
         </is>
       </c>
-      <c r="C25" s="3" t="inlineStr">
+      <c r="C25" s="2" t="inlineStr">
         <is>
           <t>Jean-pierre</t>
         </is>
       </c>
-      <c r="D25" s="3" t="inlineStr">
-        <is>
-          <t>231231JB0</t>
-        </is>
-      </c>
-      <c r="E25" s="3" t="inlineStr">
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>231231JB1</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F25" s="3" t="n"/>
-      <c r="G25" s="3" t="b">
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H25" s="3" t="inlineStr">
+      <c r="H25" s="2" t="inlineStr">
         <is>
           <t>40 rue du hamster</t>
         </is>
       </c>
-      <c r="I25" s="3" t="inlineStr">
+      <c r="I25" s="2" t="inlineStr">
         <is>
           <t>73100</t>
         </is>
       </c>
-      <c r="J25" s="3" t="inlineStr">
+      <c r="J25" s="2" t="inlineStr">
         <is>
           <t>AIX LES BAINS</t>
         </is>
       </c>
-      <c r="K25" s="3" t="inlineStr"/>
-      <c r="L25" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="3" t="inlineStr">
+      <c r="K25" s="2" t="inlineStr"/>
+      <c r="L25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R25" s="3" t="inlineStr">
+      <c r="R25" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S25" s="3" t="n"/>
+      <c r="S25" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Les reçus fiscaux sont maintenant enregistrés dans des répertoires qui correspond à la date du paiement Les reçus qui n'existent plus dans les fichiers de paiements sont supprimés du fichier .save (le PDF reste) On sauvegarde le fichier .save qu'une seule fois pour tous les reçus mis à jour/créés Correction du template pour les reçus (taille des champs + ajout d'un champ pour l'année d'édition) Correction de la découpe du nom + prénom dans les fichiers de paiements Paypal (dans le cas où le nom est composé) Début mise en place du calcul du montant (selon RAA etc)
</commit_message>
<xml_diff>
--- a/donnees/listesAdherents/2023.xlsx
+++ b/donnees/listesAdherents/2023.xlsx
@@ -625,16 +625,16 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q2" s="2" t="inlineStr">
         <is>
@@ -698,16 +698,16 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="2" t="inlineStr">
         <is>
@@ -771,16 +771,16 @@
         <v>0</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="Q4" s="2" t="inlineStr">
         <is>
@@ -844,16 +844,16 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>0</v>
+        <v>264</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="Q5" s="2" t="inlineStr">
         <is>
@@ -917,16 +917,16 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O6" s="2" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="Q6" s="2" t="inlineStr">
         <is>
@@ -990,16 +990,16 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O7" s="2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q7" s="2" t="inlineStr">
         <is>
@@ -1063,16 +1063,16 @@
         <v>0</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="O8" s="2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q8" s="2" t="inlineStr">
         <is>
@@ -1136,16 +1136,16 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="O9" s="2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="P9" s="2" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q9" s="2" t="inlineStr">
         <is>
@@ -1209,16 +1209,16 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O10" s="2" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="P10" s="2" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="Q10" s="2" t="inlineStr">
         <is>
@@ -1282,16 +1282,16 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O11" s="2" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="P11" s="2" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="Q11" s="2" t="inlineStr">
         <is>
@@ -1355,16 +1355,16 @@
         <v>0</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="O12" s="2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="P12" s="2" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q12" s="2" t="inlineStr">
         <is>
@@ -1428,16 +1428,16 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N13" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O13" s="2" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="P13" s="2" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="Q13" s="2" t="inlineStr">
         <is>
@@ -1501,16 +1501,16 @@
         <v>0</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N14" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O14" s="2" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="P14" s="2" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="Q14" s="2" t="inlineStr">
         <is>
@@ -1574,16 +1574,16 @@
         <v>0</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="O15" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P15" s="2" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q15" s="2" t="inlineStr">
         <is>
@@ -1647,16 +1647,16 @@
         <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O16" s="2" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q16" s="2" t="inlineStr">
         <is>
@@ -1720,16 +1720,16 @@
         <v>0</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N17" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O17" s="2" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="P17" s="2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q17" s="2" t="inlineStr">
         <is>
@@ -1793,16 +1793,16 @@
         <v>0</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N18" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O18" s="2" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="P18" s="2" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="Q18" s="2" t="inlineStr">
         <is>
@@ -1866,16 +1866,16 @@
         <v>0</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N19" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O19" s="2" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="P19" s="2" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="Q19" s="2" t="inlineStr">
         <is>
@@ -1939,16 +1939,16 @@
         <v>0</v>
       </c>
       <c r="M20" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N20" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O20" s="2" t="n">
-        <v>0</v>
+        <v>264</v>
       </c>
       <c r="P20" s="2" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="Q20" s="2" t="inlineStr">
         <is>
@@ -2012,16 +2012,16 @@
         <v>0</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N21" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O21" s="2" t="n">
-        <v>0</v>
+        <v>264</v>
       </c>
       <c r="P21" s="2" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="Q21" s="2" t="inlineStr">
         <is>
@@ -2085,16 +2085,16 @@
         <v>0</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N22" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O22" s="2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P22" s="2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q22" s="2" t="inlineStr">
         <is>
@@ -2158,16 +2158,16 @@
         <v>0</v>
       </c>
       <c r="M23" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N23" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O23" s="2" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="P23" s="2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q23" s="2" t="inlineStr">
         <is>
@@ -2231,16 +2231,16 @@
         <v>0</v>
       </c>
       <c r="M24" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N24" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O24" s="2" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="P24" s="2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q24" s="2" t="inlineStr">
         <is>
@@ -2304,16 +2304,16 @@
         <v>0</v>
       </c>
       <c r="M25" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N25" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O25" s="2" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="P25" s="2" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="Q25" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Montants calculés correctement Les identifiants des reçus sont maintenant bien uniques Refactorisation de plusieurs parties du code (pour mieux suivre une structure MVC) Les éventuelles notes concernant les adhérents sont bien gardés en mémoire et remis dans les listes d'adhérents Amélioration des messages warnings et erreurs Renommer certaines colonnes des fichiers Excel pour qu'elles soient moins larges Ajout d'une colonne "Régulier" pour savoir si un adhérent fait des dons régulièrement ou non Autres...
</commit_message>
<xml_diff>
--- a/donnees/listesAdherents/2023.xlsx
+++ b/donnees/listesAdherents/2023.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,22 +460,23 @@
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
     <col width="5" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
     <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="25" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="15" customWidth="1" min="11" max="11"/>
-    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="25" customWidth="1" min="9" max="9"/>
+    <col width="8" customWidth="1" min="10" max="10"/>
+    <col width="25" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
     <col width="8" customWidth="1" min="13" max="13"/>
     <col width="8" customWidth="1" min="14" max="14"/>
     <col width="8" customWidth="1" min="15" max="15"/>
     <col width="8" customWidth="1" min="16" max="16"/>
-    <col width="15" customWidth="1" min="17" max="17"/>
+    <col width="8" customWidth="1" min="17" max="17"/>
     <col width="10" customWidth="1" min="18" max="18"/>
-    <col width="20" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="20" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -491,7 +492,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Prenom</t>
+          <t>Prénom</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -506,70 +507,75 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Date dernière adhésion</t>
+          <t>Dern. adh.</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Régulier</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Envoi mails</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Adresse</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Code postal</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Ville</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Téléphone</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Montant adhésion payé année n-1</t>
-        </is>
-      </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Montant adhésion année n</t>
+          <t>Adh. 2022</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Montant adhésion année n+1</t>
+          <t>Adh. 2023</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Montant dons année n</t>
+          <t>Adh. 2024</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Total année n</t>
+          <t>Dons 2023</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Dernier paiement</t>
+          <t>Total 2023</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>Dern. paiement</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>Dern. moy. paiement</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Remarques</t>
         </is>
@@ -578,22 +584,22 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>nj76@mail.com</t>
+          <t>test@mail.com</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>CARY</t>
+          <t>COBAIN</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>André</t>
+          <t>Kurt</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>231231AC1</t>
+          <t>231002KC1</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -603,70 +609,73 @@
       </c>
       <c r="F2" s="2" t="n"/>
       <c r="G2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>17 rue du hamster</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
+          <t>1 allée Keanu Reeves</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
           <t>38000</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="K2" s="2" t="inlineStr">
         <is>
           <t>Grenoble</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr"/>
-      <c r="L2" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="L2" s="2" t="inlineStr"/>
       <c r="M2" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>124</v>
+        <v>7</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>160</v>
-      </c>
-      <c r="Q2" s="2" t="inlineStr">
-        <is>
-          <t>31/12/2023</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>25</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>helloAsso</t>
-        </is>
-      </c>
-      <c r="S2" s="2" t="n"/>
+          <t>02/10/2023</t>
+        </is>
+      </c>
+      <c r="S2" s="2" t="inlineStr">
+        <is>
+          <t>Espèce</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>joj98@mail.com</t>
+          <t>nj76@mail.com</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>TAMALOUT</t>
+          <t>CARY</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Alexandre</t>
+          <t>André</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>231231AT2</t>
+          <t>231231AC1</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
@@ -676,70 +685,73 @@
       </c>
       <c r="F3" s="2" t="n"/>
       <c r="G3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>18 rue du lapin</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
+          <t>17 rue du hamster</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
           <t>38000</t>
         </is>
       </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>GRENOBLE</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr"/>
-      <c r="L3" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>Grenoble</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr"/>
       <c r="M3" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="2" t="inlineStr">
+        <v>124</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="R3" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R3" s="2" t="inlineStr">
+      <c r="S3" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S3" s="2" t="n"/>
+      <c r="T3" s="2" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>sd78@mail.com</t>
+          <t>joj98@mail.com</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>PROVOST</t>
+          <t>TAMALOUT</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Vincent</t>
+          <t>Alexandre</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>231231VP1</t>
+          <t>231231AT1</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
@@ -749,70 +761,73 @@
       </c>
       <c r="F4" s="2" t="n"/>
       <c r="G4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="inlineStr">
-        <is>
-          <t>19 avenue du dromadaire</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
+          <t>18 rue du lapin</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
           <t>38000</t>
         </is>
       </c>
-      <c r="J4" s="2" t="inlineStr">
-        <is>
-          <t>Grenoble</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="inlineStr"/>
-      <c r="L4" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>GRENOBLE</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr"/>
       <c r="M4" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N4" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>164</v>
+        <v>18</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="Q4" s="2" t="inlineStr">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="R4" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R4" s="2" t="inlineStr">
+      <c r="S4" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S4" s="2" t="n"/>
+      <c r="T4" s="2" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>oiij78@test.fr</t>
+          <t>sd78@mail.com</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>PREVOST</t>
+          <t>PROVOST</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Arthur</t>
+          <t>Vincent</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>231231AP1</t>
+          <t>231231VP1</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
@@ -822,70 +837,73 @@
       </c>
       <c r="F5" s="2" t="n"/>
       <c r="G5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="inlineStr">
-        <is>
-          <t>20 rue du lapin</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>38340</t>
+          <t>19 avenue du dromadaire</t>
         </is>
       </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
-          <t>Voreppe</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="inlineStr"/>
-      <c r="L5" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38000</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>Grenoble</t>
+        </is>
+      </c>
+      <c r="L5" s="2" t="inlineStr"/>
       <c r="M5" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>264</v>
+        <v>18</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="Q5" s="2" t="inlineStr">
+        <v>164</v>
+      </c>
+      <c r="Q5" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="R5" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R5" s="2" t="inlineStr">
+      <c r="S5" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S5" s="2" t="n"/>
+      <c r="T5" s="2" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>mooj98@exemple.fr</t>
+          <t>oiij78@test.fr</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>JULIEN</t>
+          <t>PREVOST</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Marion</t>
+          <t>Arthur</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>231231MJ1</t>
+          <t>231231AP1</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
@@ -897,68 +915,71 @@
       <c r="G6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>21 rue de la gerbille</t>
-        </is>
+      <c r="H6" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>38440</t>
+          <t>20 rue du lapin</t>
         </is>
       </c>
       <c r="J6" s="2" t="inlineStr">
         <is>
-          <t>ARTAS</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="inlineStr"/>
-      <c r="L6" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38340</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>Voreppe</t>
+        </is>
+      </c>
+      <c r="L6" s="2" t="inlineStr"/>
       <c r="M6" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O6" s="2" t="n">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="Q6" s="2" t="inlineStr">
+        <v>264</v>
+      </c>
+      <c r="Q6" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="R6" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R6" s="2" t="inlineStr">
+      <c r="S6" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S6" s="2" t="n"/>
+      <c r="T6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>jsjs65@exemple.fr</t>
+          <t>mooj98@exemple.fr</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>MAURICE</t>
+          <t>JULIEN</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Matilda</t>
+          <t>Marion</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>231231MM1</t>
+          <t>231231MJ1</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
@@ -970,68 +991,71 @@
       <c r="G7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="2" t="inlineStr">
-        <is>
-          <t>22 rue du zèbre</t>
-        </is>
+      <c r="H7" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>38350</t>
+          <t>21 rue de la gerbille</t>
         </is>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
-          <t>Nantes en Rattier</t>
-        </is>
-      </c>
-      <c r="K7" s="2" t="inlineStr"/>
-      <c r="L7" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38440</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>ARTAS</t>
+        </is>
+      </c>
+      <c r="L7" s="2" t="inlineStr"/>
       <c r="M7" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N7" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O7" s="2" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q7" s="2" t="inlineStr">
+        <v>114</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="R7" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R7" s="2" t="inlineStr">
+      <c r="S7" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S7" s="2" t="n"/>
+      <c r="T7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>bbu756@mail.com</t>
+          <t>jsjs65@exemple.fr</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>VINCENT</t>
+          <t>MAURICE</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Véronique</t>
+          <t>Matilda</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>231231VV1</t>
+          <t>231231MM1</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
@@ -1041,70 +1065,73 @@
       </c>
       <c r="F8" s="2" t="n"/>
       <c r="G8" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>23 rue de la gerbille</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>38600</t>
+          <t>22 rue du zèbre</t>
         </is>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
-          <t>fontaine</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="inlineStr"/>
-      <c r="L8" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38350</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
+          <t>Nantes en Rattier</t>
+        </is>
+      </c>
+      <c r="L8" s="2" t="inlineStr"/>
       <c r="M8" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O8" s="2" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q8" s="2" t="inlineStr">
+        <v>14</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="R8" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R8" s="2" t="inlineStr">
+      <c r="S8" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S8" s="2" t="n"/>
+      <c r="T8" s="2" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>bbhs65@test.fr</t>
+          <t>bbu756@mail.com</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>BOULANGER</t>
+          <t>VINCENT</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Ludivine</t>
+          <t>Véronique</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>231231LB1</t>
+          <t>231231VV1</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
@@ -1114,70 +1141,73 @@
       </c>
       <c r="F9" s="2" t="n"/>
       <c r="G9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2" t="inlineStr">
-        <is>
-          <t>24 allée des lagomorphes</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>38640</t>
+          <t>23 rue de la gerbille</t>
         </is>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
-          <t>CLAIX</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="inlineStr"/>
-      <c r="L9" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38600</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>fontaine</t>
+        </is>
+      </c>
+      <c r="L9" s="2" t="inlineStr"/>
       <c r="M9" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O9" s="2" t="n">
         <v>12</v>
       </c>
       <c r="P9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q9" s="2" t="inlineStr">
+      <c r="R9" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R9" s="2" t="inlineStr">
+      <c r="S9" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S9" s="2" t="n"/>
+      <c r="T9" s="2" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>hdhc8@exemple.fr</t>
+          <t>bbhs65@test.fr</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>PASTEUR</t>
+          <t>BOULANGER</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Thérèse</t>
+          <t>Ludivine</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>231231TP1</t>
+          <t>231231LB1</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
@@ -1187,70 +1217,73 @@
       </c>
       <c r="F10" s="2" t="n"/>
       <c r="G10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>25 rue du capybara</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>38600</t>
+          <t>24 allée des lagomorphes</t>
         </is>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
-          <t>Fontaine</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="inlineStr"/>
-      <c r="L10" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38640</t>
+        </is>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>CLAIX</t>
+        </is>
+      </c>
+      <c r="L10" s="2" t="inlineStr"/>
       <c r="M10" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O10" s="2" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="P10" s="2" t="n">
-        <v>55</v>
-      </c>
-      <c r="Q10" s="2" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="R10" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R10" s="2" t="inlineStr">
+      <c r="S10" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S10" s="2" t="n"/>
+      <c r="T10" s="2" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>jnjsd7@test.fr</t>
+          <t>hdhc8@exemple.fr</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>PASTIER</t>
+          <t>PASTEUR</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Jean-pierre</t>
+          <t>Thérèse</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>231231JP1</t>
+          <t>231231TP1</t>
         </is>
       </c>
       <c r="E11" s="2" t="inlineStr">
@@ -1260,70 +1293,73 @@
       </c>
       <c r="F11" s="2" t="n"/>
       <c r="G11" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>26 avenue du dromadaire</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I11" s="2" t="inlineStr">
         <is>
-          <t>73700</t>
+          <t>25 rue du capybara</t>
         </is>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
-          <t>SEEZ</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="inlineStr"/>
-      <c r="L11" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38600</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>Fontaine</t>
+        </is>
+      </c>
+      <c r="L11" s="2" t="inlineStr"/>
       <c r="M11" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O11" s="2" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="P11" s="2" t="n">
-        <v>72</v>
-      </c>
-      <c r="Q11" s="2" t="inlineStr">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="R11" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R11" s="2" t="inlineStr">
+      <c r="S11" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S11" s="2" t="n"/>
+      <c r="T11" s="2" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>jbjsbd8@exemple.fr</t>
+          <t>jnjsd7@test.fr</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>RUCHER</t>
+          <t>PASTIER</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>Jean-pierre</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>231231FR1</t>
+          <t>231231JP1</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
@@ -1335,68 +1371,71 @@
       <c r="G12" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="2" t="inlineStr">
-        <is>
-          <t>27 rue du lapin</t>
-        </is>
+      <c r="H12" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I12" s="2" t="inlineStr">
         <is>
-          <t>38920</t>
+          <t>26 avenue du dromadaire</t>
         </is>
       </c>
       <c r="J12" s="2" t="inlineStr">
         <is>
-          <t>Crolles</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="inlineStr"/>
-      <c r="L12" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>73700</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>SEEZ</t>
+        </is>
+      </c>
+      <c r="L12" s="2" t="inlineStr"/>
       <c r="M12" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O12" s="2" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="P12" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q12" s="2" t="inlineStr">
+        <v>36</v>
+      </c>
+      <c r="Q12" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="R12" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R12" s="2" t="inlineStr">
+      <c r="S12" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S12" s="2" t="n"/>
+      <c r="T12" s="2" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>sjdbj786@exemple.fr</t>
+          <t>jbjsbd8@exemple.fr</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>TISON</t>
+          <t>RUCHER</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Gisèle</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>231231GT1</t>
+          <t>231231FR1</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
@@ -1406,70 +1445,73 @@
       </c>
       <c r="F13" s="2" t="n"/>
       <c r="G13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2" t="inlineStr">
-        <is>
-          <t>28 allée des lagomorphes</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I13" s="2" t="inlineStr">
         <is>
-          <t>38190</t>
+          <t>27 rue du lapin</t>
         </is>
       </c>
       <c r="J13" s="2" t="inlineStr">
         <is>
-          <t>LAVAL</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="inlineStr"/>
-      <c r="L13" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38920</t>
+        </is>
+      </c>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>Crolles</t>
+        </is>
+      </c>
+      <c r="L13" s="2" t="inlineStr"/>
       <c r="M13" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O13" s="2" t="n">
-        <v>114</v>
+        <v>12</v>
       </c>
       <c r="P13" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="Q13" s="2" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="R13" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R13" s="2" t="inlineStr">
+      <c r="S13" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S13" s="2" t="n"/>
+      <c r="T13" s="2" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>bhsd112@test.fr</t>
+          <t>sjdbj786@exemple.fr</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>TRESSEAU</t>
+          <t>TISON</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Yves</t>
+          <t>Gisèle</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>231231YT1</t>
+          <t>231231GT1</t>
         </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
@@ -1479,70 +1521,73 @@
       </c>
       <c r="F14" s="2" t="n"/>
       <c r="G14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2" t="inlineStr">
-        <is>
-          <t>29 rue du zèbre</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I14" s="2" t="inlineStr">
         <is>
-          <t>38360</t>
+          <t>28 allée des lagomorphes</t>
         </is>
       </c>
       <c r="J14" s="2" t="inlineStr">
         <is>
-          <t>Noyarey</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="inlineStr"/>
-      <c r="L14" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38190</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
+          <t>LAVAL</t>
+        </is>
+      </c>
+      <c r="L14" s="2" t="inlineStr"/>
       <c r="M14" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O14" s="2" t="n">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="P14" s="2" t="n">
-        <v>80</v>
-      </c>
-      <c r="Q14" s="2" t="inlineStr">
+        <v>114</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="R14" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R14" s="2" t="inlineStr">
+      <c r="S14" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S14" s="2" t="n"/>
+      <c r="T14" s="2" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>jij134@exemple.fr</t>
+          <t>bhsd112@test.fr</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>MORGAN</t>
+          <t>TRESSEAU</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Gilles</t>
+          <t>Yves</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>231231GM1</t>
+          <t>231231YT1</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
@@ -1552,70 +1597,73 @@
       </c>
       <c r="F15" s="2" t="n"/>
       <c r="G15" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2" t="inlineStr">
-        <is>
-          <t>30 rue du lapin</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I15" s="2" t="inlineStr">
         <is>
-          <t>38600</t>
+          <t>29 rue du zèbre</t>
         </is>
       </c>
       <c r="J15" s="2" t="inlineStr">
         <is>
-          <t>FONTAINE</t>
-        </is>
-      </c>
-      <c r="K15" s="2" t="inlineStr"/>
-      <c r="L15" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38360</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="inlineStr">
+        <is>
+          <t>Noyarey</t>
+        </is>
+      </c>
+      <c r="L15" s="2" t="inlineStr"/>
       <c r="M15" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N15" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O15" s="2" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="P15" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q15" s="2" t="inlineStr">
+        <v>44</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="R15" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R15" s="2" t="inlineStr">
+      <c r="S15" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S15" s="2" t="n"/>
+      <c r="T15" s="2" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>hu7651@test.fr</t>
+          <t>jij134@exemple.fr</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>LECLERC</t>
+          <t>MORGAN</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>Léa</t>
+          <t>Gilles</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>231231LL1</t>
+          <t>231231GM1</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
@@ -1625,70 +1673,73 @@
       </c>
       <c r="F16" s="2" t="n"/>
       <c r="G16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2" t="inlineStr">
-        <is>
-          <t>31 rue de la gerbille</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I16" s="2" t="inlineStr">
         <is>
-          <t>38610</t>
+          <t>30 rue du lapin</t>
         </is>
       </c>
       <c r="J16" s="2" t="inlineStr">
         <is>
-          <t>Gières</t>
-        </is>
-      </c>
-      <c r="K16" s="2" t="inlineStr"/>
-      <c r="L16" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38600</t>
+        </is>
+      </c>
+      <c r="K16" s="2" t="inlineStr">
+        <is>
+          <t>FONTAINE</t>
+        </is>
+      </c>
+      <c r="L16" s="2" t="inlineStr"/>
       <c r="M16" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O16" s="2" t="n">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q16" s="2" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="R16" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R16" s="2" t="inlineStr">
+      <c r="S16" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S16" s="2" t="n"/>
+      <c r="T16" s="2" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>12djd@mail.com</t>
+          <t>hu7651@test.fr</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>SOLOGNOT</t>
+          <t>LECLERC</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Léo</t>
+          <t>Léa</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>231231LS1</t>
+          <t>231231LL1</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
@@ -1698,70 +1749,73 @@
       </c>
       <c r="F17" s="2" t="n"/>
       <c r="G17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2" t="inlineStr">
-        <is>
-          <t>32 rue du zèbre</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H17" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I17" s="2" t="inlineStr">
         <is>
-          <t>69230</t>
+          <t>31 rue de la gerbille</t>
         </is>
       </c>
       <c r="J17" s="2" t="inlineStr">
         <is>
-          <t>SAINT-GENIS-LAVAL</t>
-        </is>
-      </c>
-      <c r="K17" s="2" t="inlineStr"/>
-      <c r="L17" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38610</t>
+        </is>
+      </c>
+      <c r="K17" s="2" t="inlineStr">
+        <is>
+          <t>Gières</t>
+        </is>
+      </c>
+      <c r="L17" s="2" t="inlineStr"/>
       <c r="M17" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N17" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O17" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="P17" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="P17" s="2" t="n">
+      <c r="Q17" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="Q17" s="2" t="inlineStr">
+      <c r="R17" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R17" s="2" t="inlineStr">
+      <c r="S17" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S17" s="2" t="n"/>
+      <c r="T17" s="2" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>091ssj@exemple.fr</t>
+          <t>12djd@mail.com</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>ZANZIBAR</t>
+          <t>SOLOGNOT</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Maurice</t>
+          <t>Léo</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>231231MZ1</t>
+          <t>231231LS1</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
@@ -1771,70 +1825,73 @@
       </c>
       <c r="F18" s="2" t="n"/>
       <c r="G18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2" t="inlineStr">
-        <is>
-          <t>33 rue de la gerbille</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I18" s="2" t="inlineStr">
         <is>
-          <t>38110</t>
+          <t>32 rue du zèbre</t>
         </is>
       </c>
       <c r="J18" s="2" t="inlineStr">
         <is>
-          <t>MONTAGNIEU</t>
-        </is>
-      </c>
-      <c r="K18" s="2" t="inlineStr"/>
-      <c r="L18" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>69230</t>
+        </is>
+      </c>
+      <c r="K18" s="2" t="inlineStr">
+        <is>
+          <t>SAINT-GENIS-LAVAL</t>
+        </is>
+      </c>
+      <c r="L18" s="2" t="inlineStr"/>
       <c r="M18" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N18" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O18" s="2" t="n">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="P18" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="Q18" s="2" t="inlineStr">
+        <v>64</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="R18" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R18" s="2" t="inlineStr">
+      <c r="S18" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S18" s="2" t="n"/>
+      <c r="T18" s="2" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>art134@mail.com</t>
+          <t>091ssj@exemple.fr</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>NORMAL</t>
+          <t>ZANZIBAR</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Patrice</t>
+          <t>Maurice</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>231231PN1</t>
+          <t>231231MZ1</t>
         </is>
       </c>
       <c r="E19" s="2" t="inlineStr">
@@ -1844,70 +1901,73 @@
       </c>
       <c r="F19" s="2" t="n"/>
       <c r="G19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" s="2" t="inlineStr">
-        <is>
-          <t>34 rue du lapin</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H19" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I19" s="2" t="inlineStr">
         <is>
-          <t>38120</t>
+          <t>33 rue de la gerbille</t>
         </is>
       </c>
       <c r="J19" s="2" t="inlineStr">
         <is>
-          <t>Saint-Égrève</t>
-        </is>
-      </c>
-      <c r="K19" s="2" t="inlineStr"/>
-      <c r="L19" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38110</t>
+        </is>
+      </c>
+      <c r="K19" s="2" t="inlineStr">
+        <is>
+          <t>MONTAGNIEU</t>
+        </is>
+      </c>
+      <c r="L19" s="2" t="inlineStr"/>
       <c r="M19" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N19" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="P19" s="2" t="n">
         <v>114</v>
       </c>
-      <c r="P19" s="2" t="n">
+      <c r="Q19" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="Q19" s="2" t="inlineStr">
+      <c r="R19" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R19" s="2" t="inlineStr">
+      <c r="S19" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S19" s="2" t="n"/>
+      <c r="T19" s="2" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>112ssss@mail.com</t>
+          <t>art134@mail.com</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>FROID</t>
+          <t>NORMAL</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Patrice</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>231231PF1</t>
+          <t>231231PN1</t>
         </is>
       </c>
       <c r="E20" s="2" t="inlineStr">
@@ -1917,70 +1977,73 @@
       </c>
       <c r="F20" s="2" t="n"/>
       <c r="G20" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2" t="inlineStr">
-        <is>
-          <t>35 avenue du dromadaire</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I20" s="2" t="inlineStr">
         <is>
-          <t>38150</t>
+          <t>34 rue du lapin</t>
         </is>
       </c>
       <c r="J20" s="2" t="inlineStr">
         <is>
-          <t>Salaise-sur-Sanne 38150</t>
-        </is>
-      </c>
-      <c r="K20" s="2" t="inlineStr"/>
-      <c r="L20" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38120</t>
+        </is>
+      </c>
+      <c r="K20" s="2" t="inlineStr">
+        <is>
+          <t>Saint-Égrève</t>
+        </is>
+      </c>
+      <c r="L20" s="2" t="inlineStr"/>
       <c r="M20" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N20" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O20" s="2" t="n">
-        <v>264</v>
+        <v>18</v>
       </c>
       <c r="P20" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="Q20" s="2" t="inlineStr">
+        <v>114</v>
+      </c>
+      <c r="Q20" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="R20" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R20" s="2" t="inlineStr">
+      <c r="S20" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S20" s="2" t="n"/>
+      <c r="T20" s="2" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>uhu761@test.fr</t>
+          <t>112ssss@mail.com</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>CHAUD</t>
+          <t>FROID</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Henri</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>231231HC1</t>
+          <t>231231PF1</t>
         </is>
       </c>
       <c r="E21" s="2" t="inlineStr">
@@ -1990,70 +2053,73 @@
       </c>
       <c r="F21" s="2" t="n"/>
       <c r="G21" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2" t="inlineStr">
-        <is>
-          <t>36 rue du hamster</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I21" s="2" t="inlineStr">
         <is>
-          <t>38300</t>
+          <t>35 avenue du dromadaire</t>
         </is>
       </c>
       <c r="J21" s="2" t="inlineStr">
         <is>
-          <t>BOURGOIN JALLIEU</t>
-        </is>
-      </c>
-      <c r="K21" s="2" t="inlineStr"/>
-      <c r="L21" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38150</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="inlineStr">
+        <is>
+          <t>Salaise-sur-Sanne 38150</t>
+        </is>
+      </c>
+      <c r="L21" s="2" t="inlineStr"/>
       <c r="M21" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N21" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O21" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="P21" s="2" t="n">
         <v>264</v>
       </c>
-      <c r="P21" s="2" t="n">
+      <c r="Q21" s="2" t="n">
         <v>300</v>
       </c>
-      <c r="Q21" s="2" t="inlineStr">
+      <c r="R21" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R21" s="2" t="inlineStr">
+      <c r="S21" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S21" s="2" t="n"/>
+      <c r="T21" s="2" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>azaz541@test.fr</t>
+          <t>uhu761@test.fr</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>TIÈDE</t>
+          <t>CHAUD</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Alice</t>
+          <t>Henri</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>231231AT1</t>
+          <t>231231HC1</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
@@ -2063,70 +2129,73 @@
       </c>
       <c r="F22" s="2" t="n"/>
       <c r="G22" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>37 rue du lapin</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H22" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I22" s="2" t="inlineStr">
         <is>
-          <t>38610</t>
+          <t>36 rue du hamster</t>
         </is>
       </c>
       <c r="J22" s="2" t="inlineStr">
         <is>
-          <t>Gieres</t>
-        </is>
-      </c>
-      <c r="K22" s="2" t="inlineStr"/>
-      <c r="L22" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38300</t>
+        </is>
+      </c>
+      <c r="K22" s="2" t="inlineStr">
+        <is>
+          <t>BOURGOIN JALLIEU</t>
+        </is>
+      </c>
+      <c r="L22" s="2" t="inlineStr"/>
       <c r="M22" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O22" s="2" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="P22" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q22" s="2" t="inlineStr">
+        <v>264</v>
+      </c>
+      <c r="Q22" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="R22" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R22" s="2" t="inlineStr">
+      <c r="S22" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S22" s="2" t="n"/>
+      <c r="T22" s="2" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>sjjs183@mail.com</t>
+          <t>azaz541@test.fr</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>TEMPERET</t>
+          <t>TIÈDE</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Véronique</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>231231VT1</t>
+          <t>231231AT2</t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr">
@@ -2136,70 +2205,73 @@
       </c>
       <c r="F23" s="2" t="n"/>
       <c r="G23" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" s="2" t="inlineStr">
-        <is>
-          <t>38 rue du capybara</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I23" s="2" t="inlineStr">
         <is>
-          <t>38000</t>
+          <t>37 rue du lapin</t>
         </is>
       </c>
       <c r="J23" s="2" t="inlineStr">
         <is>
-          <t>GRENOBLE</t>
-        </is>
-      </c>
-      <c r="K23" s="2" t="inlineStr"/>
-      <c r="L23" s="2" t="n">
-        <v>0</v>
-      </c>
+          <t>38610</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="inlineStr">
+        <is>
+          <t>Gieres</t>
+        </is>
+      </c>
+      <c r="L23" s="2" t="inlineStr"/>
       <c r="M23" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N23" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O23" s="2" t="n">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="P23" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q23" s="2" t="inlineStr">
+        <v>14</v>
+      </c>
+      <c r="Q23" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="R23" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R23" s="2" t="inlineStr">
+      <c r="S23" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S23" s="2" t="n"/>
+      <c r="T23" s="2" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>apn514@mail.com</t>
+          <t>sjjs183@mail.com</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>PARASOL</t>
+          <t>TEMPERET</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>Nathalie</t>
+          <t>Véronique</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>231231NP1</t>
+          <t>231231VT1</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
@@ -2209,70 +2281,73 @@
       </c>
       <c r="F24" s="2" t="n"/>
       <c r="G24" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" s="2" t="inlineStr">
-        <is>
-          <t>39 rue de la gerbille</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I24" s="2" t="inlineStr">
         <is>
+          <t>38 rue du capybara</t>
+        </is>
+      </c>
+      <c r="J24" s="2" t="inlineStr">
+        <is>
           <t>38000</t>
         </is>
       </c>
-      <c r="J24" s="2" t="inlineStr">
+      <c r="K24" s="2" t="inlineStr">
         <is>
           <t>GRENOBLE</t>
         </is>
       </c>
-      <c r="K24" s="2" t="inlineStr"/>
-      <c r="L24" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="L24" s="2" t="inlineStr"/>
       <c r="M24" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N24" s="2" t="n">
         <v>18</v>
       </c>
       <c r="O24" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="P24" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="P24" s="2" t="n">
+      <c r="Q24" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="Q24" s="2" t="inlineStr">
+      <c r="R24" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R24" s="2" t="inlineStr">
+      <c r="S24" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S24" s="2" t="n"/>
+      <c r="T24" s="2" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>jijsq12@mail.com</t>
+          <t>apn514@mail.com</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>BAIGNOIRE</t>
+          <t>PARASOL</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>Jean-pierre</t>
+          <t>Nathalie</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>231231JB1</t>
+          <t>231231NP1</t>
         </is>
       </c>
       <c r="E25" s="2" t="inlineStr">
@@ -2282,50 +2357,129 @@
       </c>
       <c r="F25" s="2" t="n"/>
       <c r="G25" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" s="2" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2" t="inlineStr">
+        <is>
+          <t>39 rue de la gerbille</t>
+        </is>
+      </c>
+      <c r="J25" s="2" t="inlineStr">
+        <is>
+          <t>38000</t>
+        </is>
+      </c>
+      <c r="K25" s="2" t="inlineStr">
+        <is>
+          <t>GRENOBLE</t>
+        </is>
+      </c>
+      <c r="L25" s="2" t="inlineStr"/>
+      <c r="M25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="O25" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="P25" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="Q25" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="R25" s="2" t="inlineStr">
+        <is>
+          <t>31/12/2023</t>
+        </is>
+      </c>
+      <c r="S25" s="2" t="inlineStr">
+        <is>
+          <t>helloAsso</t>
+        </is>
+      </c>
+      <c r="T25" s="2" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>jijsq12@mail.com</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>BAIGNOIRE</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>Jean-pierre</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>231231JB1</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="n"/>
+      <c r="G26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="inlineStr">
         <is>
           <t>40 rue du hamster</t>
         </is>
       </c>
-      <c r="I25" s="2" t="inlineStr">
+      <c r="J26" s="2" t="inlineStr">
         <is>
           <t>73100</t>
         </is>
       </c>
-      <c r="J25" s="2" t="inlineStr">
+      <c r="K26" s="2" t="inlineStr">
         <is>
           <t>AIX LES BAINS</t>
         </is>
       </c>
-      <c r="K25" s="2" t="inlineStr"/>
-      <c r="L25" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="N25" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="O25" s="2" t="n">
+      <c r="L26" s="2" t="inlineStr"/>
+      <c r="M26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="O26" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="P26" s="2" t="n">
         <v>114</v>
       </c>
-      <c r="P25" s="2" t="n">
+      <c r="Q26" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="Q25" s="2" t="inlineStr">
+      <c r="R26" s="2" t="inlineStr">
         <is>
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="R25" s="2" t="inlineStr">
+      <c r="S26" s="2" t="inlineStr">
         <is>
           <t>helloAsso</t>
         </is>
       </c>
-      <c r="S25" s="2" t="n"/>
+      <c r="T26" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactorisation selon modèle MVC complétée Divers bugs corrigés Premier onglet (mise à jour) fonctionnel Début deuxième onglet (reçus fiscaux) Autres...
</commit_message>
<xml_diff>
--- a/donnees/listesAdherents/2023.xlsx
+++ b/donnees/listesAdherents/2023.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <col width="8" customWidth="1" min="14" max="14"/>
     <col width="8" customWidth="1" min="15" max="15"/>
     <col width="8" customWidth="1" min="16" max="16"/>
-    <col width="8" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
     <col width="10" customWidth="1" min="18" max="18"/>
     <col width="10" customWidth="1" min="19" max="19"/>
     <col width="20" customWidth="1" min="20" max="20"/>
@@ -604,7 +604,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
@@ -680,7 +680,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -756,7 +756,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F4" s="2" t="n"/>
@@ -832,7 +832,7 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F5" s="2" t="n"/>
@@ -908,7 +908,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F6" s="2" t="n"/>
@@ -984,7 +984,7 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F7" s="2" t="n"/>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F9" s="2" t="n"/>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F10" s="2" t="n"/>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F11" s="2" t="n"/>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F12" s="2" t="n"/>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F13" s="2" t="n"/>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F14" s="2" t="n"/>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F15" s="2" t="n"/>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F16" s="2" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F17" s="2" t="n"/>
@@ -1820,7 +1820,7 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F18" s="2" t="n"/>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F19" s="2" t="n"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F20" s="2" t="n"/>
@@ -2048,7 +2048,7 @@
       </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F21" s="2" t="n"/>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F22" s="2" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F23" s="2" t="n"/>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F24" s="2" t="n"/>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F25" s="2" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>RAA</t>
         </is>
       </c>
       <c r="F26" s="2" t="n"/>
@@ -2480,6 +2480,112 @@
         </is>
       </c>
       <c r="T26" s="2" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n"/>
+      <c r="B27" s="2" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n"/>
+      <c r="E27" s="2" t="n"/>
+      <c r="F27" s="2" t="n"/>
+      <c r="G27" s="2" t="n"/>
+      <c r="H27" s="2" t="n"/>
+      <c r="I27" s="2" t="n"/>
+      <c r="J27" s="2" t="n"/>
+      <c r="K27" s="2" t="n"/>
+      <c r="L27" s="2" t="n"/>
+      <c r="M27" s="2" t="n"/>
+      <c r="N27" s="2" t="n"/>
+      <c r="O27" s="2" t="n"/>
+      <c r="P27" s="2" t="n"/>
+      <c r="Q27" s="2" t="n"/>
+      <c r="R27" s="2" t="n"/>
+      <c r="S27" s="2" t="n"/>
+      <c r="T27" s="2" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>Nombre de reçus</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="C28" s="2" t="n"/>
+      <c r="D28" s="2" t="n"/>
+      <c r="E28" s="2" t="n"/>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="2" t="n"/>
+      <c r="H28" s="2" t="n"/>
+      <c r="I28" s="2" t="n"/>
+      <c r="J28" s="2" t="n"/>
+      <c r="K28" s="2" t="n"/>
+      <c r="L28" s="2" t="n"/>
+      <c r="M28" s="2" t="n"/>
+      <c r="N28" s="2" t="n"/>
+      <c r="O28" s="2" t="n"/>
+      <c r="P28" s="2" t="n"/>
+      <c r="Q28" s="2" t="n"/>
+      <c r="R28" s="2" t="n"/>
+      <c r="S28" s="2" t="n"/>
+      <c r="T28" s="2" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>Total avec reçus</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>2902</v>
+      </c>
+      <c r="C29" s="2" t="n"/>
+      <c r="D29" s="2" t="n"/>
+      <c r="E29" s="2" t="n"/>
+      <c r="F29" s="2" t="n"/>
+      <c r="G29" s="2" t="n"/>
+      <c r="H29" s="2" t="n"/>
+      <c r="I29" s="2" t="n"/>
+      <c r="J29" s="2" t="n"/>
+      <c r="K29" s="2" t="n"/>
+      <c r="L29" s="2" t="n"/>
+      <c r="M29" s="2" t="n"/>
+      <c r="N29" s="2" t="n"/>
+      <c r="O29" s="2" t="n"/>
+      <c r="P29" s="2" t="n"/>
+      <c r="Q29" s="2" t="n"/>
+      <c r="R29" s="2" t="n"/>
+      <c r="S29" s="2" t="n"/>
+      <c r="T29" s="2" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Total sans reçus</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2" t="n"/>
+      <c r="D30" s="2" t="n"/>
+      <c r="E30" s="2" t="n"/>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="2" t="n"/>
+      <c r="H30" s="2" t="n"/>
+      <c r="I30" s="2" t="n"/>
+      <c r="J30" s="2" t="n"/>
+      <c r="K30" s="2" t="n"/>
+      <c r="L30" s="2" t="n"/>
+      <c r="M30" s="2" t="n"/>
+      <c r="N30" s="2" t="n"/>
+      <c r="O30" s="2" t="n"/>
+      <c r="P30" s="2" t="n"/>
+      <c r="Q30" s="2" t="n"/>
+      <c r="R30" s="2" t="n"/>
+      <c r="S30" s="2" t="n"/>
+      <c r="T30" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Pas mal de nouveautés... Que j'ai pas noté.
</commit_message>
<xml_diff>
--- a/donnees/listesAdherents/2023.xlsx
+++ b/donnees/listesAdherents/2023.xlsx
@@ -921,12 +921,12 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>231231AP1</t>
+          <t>231231APR1</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>RAA</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F6" s="2" t="n"/>
@@ -959,10 +959,10 @@
         <v>18</v>
       </c>
       <c r="O6" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="Q6" s="2" t="n">
         <v>300</v>
@@ -1000,12 +1000,12 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>231231MJ1</t>
+          <t>231231MJR1</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>RAA</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F7" s="2" t="n"/>
@@ -1038,10 +1038,10 @@
         <v>18</v>
       </c>
       <c r="O7" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="Q7" s="2" t="n">
         <v>150</v>
@@ -1395,12 +1395,12 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>231231JP1</t>
+          <t>231231JPR1</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>RAA</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F12" s="2" t="n"/>
@@ -1433,10 +1433,10 @@
         <v>18</v>
       </c>
       <c r="O12" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="P12" s="2" t="n">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="Q12" s="2" t="n">
         <v>72</v>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>231231AT2</t>
+          <t>231231AT1</t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr">

</xml_diff>